<commit_message>
Realização da Simulação TB
Neste commit tem-se a simulação por turning bands e as realizações obtidas.
</commit_message>
<xml_diff>
--- a/Turning Bands/Variogramas/TB_Variograms.xlsx
+++ b/Turning Bands/Variogramas/TB_Variograms.xlsx
@@ -371,7 +371,7 @@
   <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
+      <selection pane="topLeft" activeCell="B45" activeCellId="0" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -745,7 +745,7 @@
         <v>17</v>
       </c>
       <c r="B45" s="4" t="n">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>